<commit_message>
added some operator(binary and unary) counter for efficiency for all 3 languages
</commit_message>
<xml_diff>
--- a/smartcodelab-datasets/CppCodes.xlsx
+++ b/smartcodelab-datasets/CppCodes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magno\OneDrive\Desktop\Capstone 2\2025-CP_SMARTCODELAB\smartcodelab-datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FA41FB-D6BE-4889-84A9-5687BACE57AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,1074 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+  <si>
+    <t>Programming Exercises</t>
+  </si>
+  <si>
+    <t>AI Generated Codes with Standards Violation</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;vector&gt; // readability-duplicate-include
+using namespace std; // readability-identifier-naming
+vector&lt;int&gt; po(vector&lt;int&gt; d) { // readability-identifier-length
+    int c = 1; // readability-identifier-length
+    for (int i = d.size() - 1; i &gt;= 0 &amp;&amp; c; i--) // readability-math-missing-parentheses
+        if (d[i] + c &gt; 9) // readability-braces-around-statements
+            d[i] = 0, c = 1; // readability-misleading-indentation
+        else 
+            d[i] = d[i] + c, c = 0; // readability-else-after-return
+    if (c == 1) // readability-magic-numbers
+        d.insert(d.begin(), c); 
+    return d; return d; // readability-redundant-control-flow
+}</t>
+  </si>
+  <si>
+    <t>You are given a large integer represented as an integer array digits, where each digits[i] is the ith digit of the integer. The digits are ordered from most significant to least significant in left-to-right order. The large integer does not contain any leading 0's.
+Increment the large integer by one and return the resulting array of digits.
+Example 1:
+Input: digits = [1,2,3]
+Output: [1,2,4]
+Explanation: The array represents the integer 123.
+Incrementing by one gives 123 + 1 = 124.
+Thus, the result should be [1,2,4].</t>
+  </si>
+  <si>
+    <t>Readability
+readability-duplicate-include
+readability-identifier-length
+readability-identifier-naming
+readability-math-missing-parentheses
+readability-braces-around-statements
+readability-misleading-indentation
+readability-else-after-return
+readability-magic-numbers
+readability-redundant-control-flow
+Maintainability
+(none)
+Robustness
+(none)</t>
+  </si>
+  <si>
+    <t>Given a m x n grid filled with non-negative numbers, find a path from top left to bottom right, which minimizes the sum of all numbers along its path.
+Note: You can only move either down or right at any point in time.
+Example 1:
+Input: grid = [[1,3,1],[1,5,1],[4,2,1]]
+Output: 7
+Explanation: Because the path 1 → 3 → 1 → 1 → 1 minimizes the sum.</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;algorithm&gt;
+#include &lt;algorithm&gt; // readability-duplicate-include
+using namespace std; // readability-identifier-naming
+int mps(vector&lt;vector&lt;int&gt;&gt;&amp; g) { // readability-identifier-length
+    int r = g.size(); // readability-identifier-length
+    int c = g[0].size(); // readability-identifier-length
+    for (int i = 1; i &lt; r; i++) // readability-magic-numbers
+        g[i][0] += g[i - 1][0]; // readability-braces-around-statements
+    for (int j = 1; j &lt; c; j++) // readability-magic-numbers
+        g[0][j] += g[0][j - 1]; // readability-braces-around-statements
+    for (int i = 1; i &lt; r; i++)
+        for (int j = 1; j &lt; c; j++)
+            g[i][j] += min(g[i - 1][j], g[i][j - 1]); // readability-misleading-indentation
+    return g[r - 1][c - 1]; return g[r - 1][c - 1]; // readability-redundant-control-flow
+}</t>
+  </si>
+  <si>
+    <t>Readability
+readability-duplicate-include
+readability-identifier-length
+readability-identifier-naming
+readability-magic-numbers
+readability-braces-around-statements
+readability-misleading-indentation
+readability-redundant-control-flow
+Maintainability
+(none)
+Robustness
+(none)</t>
+  </si>
+  <si>
+    <t>You are given an array of non-overlapping intervals intervals where intervals[i] = [starti, endi] represent the start and the end of the ith interval and intervals is sorted in ascending order by starti. You are also given an interval newInterval = [start, end] that represents the start and end of another interval.
+Insert newInterval into intervals such that intervals is still sorted in ascending order by starti and intervals still does not have any overlapping intervals (merge overlapping intervals if necessary).
+Return intervals after the insertion.
+Note that you don't need to modify intervals in-place. You can make a new array and return it.
+Example 1:
+Input: intervals = [[1,3],[6,9]], newInterval = [2,5]
+Output: [[1,5],[6,9]]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-duplicate-include
+readability-identifier-length
+readability-identifier-naming
+readability-math-missing-parentheses
+readability-braces-around-statements
+readability-misleading-indentation
+readability-magic-numbers
+readability-redundant-control-flow
+Maintainability
+(none)
+Robustness
+(none)</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;vector&gt; // readability-duplicate-include
+using namespace std; // readability-identifier-naming
+vector&lt;vector&lt;int&gt;&gt; ins(vector&lt;vector&lt;int&gt;&gt;&amp; iv, vector&lt;int&gt;&amp; ni) { // readability-identifier-length
+    vector&lt;vector&lt;int&gt;&gt; r; // readability-identifier-length
+    int i = 0; // readability-identifier-length
+    int n = iv.size(); // readability-identifier-length
+    while (i &lt; n &amp;&amp; iv[i][1] &lt; ni[0]) // readability-math-missing-parentheses
+        r.push_back(iv[i++]); // readability-braces-around-statements
+    while (i &lt; n &amp;&amp; iv[i][0] &lt;= ni[1]) // readability-math-missing-parentheses
+        ni[0] = min(ni[0], iv[i][0]), ni[1] = max(ni[1], iv[i][1]), i++; // readability-misleading-indentation, readability-magic-numbers
+    r.push_back(ni);
+    while (i &lt; n)
+        r.push_back(iv[i++]); // readability-braces-around-statements
+    return r; return r; // readability-redundant-control-flow
+}</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-control-flow
+readability-implicit-bool-conversion
+readability-function-cognitive-complexity
+readability-braces-around-statements
+Maintainability
+readability-simplify-boolean-expr
+Robustness
+bugprone-integer-division
+misc-unused-parameters</t>
+  </si>
+  <si>
+    <t>Given an array of intervals where intervals[i] = [starti, endi], merge all overlapping intervals, and return an array of the non-overlapping intervals that cover all the intervals in the input.
+Example 1:
+Input: intervals = [[1,3],[2,6],[8,10],[15,18]]
+Output: [[1,6],[8,10],[15,18]]
+Explanation: Since intervals [1,3] and [2,6] overlap, merge them into [1,6].</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;algorithm&gt;
+using namespace std;
+class Solution {
+public:
+    vector&lt;vector&lt;int&gt;&gt; merge(vector&lt;vector&lt;int&gt;&gt;&amp; i) {  // readability-identifier-length
+        if (i.empty()) return {};
+        sort(i.begin(), i.end());
+        vector&lt;vector&lt;int&gt;&gt; result;
+        result.push_back(i[0]);
+        for (int x = 1; x &lt; i.size(); x++) {  // readability-identifier-length
+            auto&amp; last = result.back();
+            auto&amp; curr = i[x];
+            if (curr[0] &lt;= last[1]) {
+                last[1] = max(last[1], curr[1]);
+            } else {
+                result.push_back(curr);
+            }
+        }
+        return result;
+    }
+    // readability-redundant-control-flow
+    void process() {
+        int a = 5;  // readability-magic-numbers
+        return;  // redundant return in void function
+    }
+    // readability-implicit-bool-conversion
+    bool check() {
+        int num = 5;
+        return num;  // implicit bool conversion
+    }
+};</t>
+  </si>
+  <si>
+    <t>You are given an integer array nums. You are initially positioned at the array's first index, and each element in the array represents your maximum jump length at that position.
+Return true if you can reach the last index, or false otherwise.
+Example 1:
+Input: nums = [2,3,1,1,4]
+Output: true
+Explanation: Jump 1 step from index 0 to 1, then 3 steps to the last index.</t>
+  </si>
+  <si>
+    <t>class Solution {
+public:
+    bool canJump(vector&lt;int&gt;&amp; n) {  // readability-identifier-length
+        int m = 0;  // readability-identifier-length
+        for (int i = 0; i &lt; n.size(); i++) {  // readability-identifier-length
+            if (i &gt; m) return false;
+            m = max(m, i + n[i]);
+            if (m &gt;= n.size() - 1) return true;
+        }
+        return false;
+    }
+    // readability-redundant-control-flow
+    void helper() {
+        int x = 5;  // readability-magic-numbers
+        return;
+    }
+    // readability-implicit-bool-conversion
+    bool check() {
+        int val = 1;  // readability-magic-numbers
+        return val;
+    }
+    // readability-else-after-return
+    bool validate(int a) {
+        if (a &gt; 10) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+};</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-control-flow
+readability-implicit-bool-conversion
+readability-else-after-return
+Maintainability
+readability-simplify-boolean-expr
+Robustness
+misc-unused-parameters</t>
+  </si>
+  <si>
+    <t>Given an integer array nums, find the subarray
+with the largest sum, and return its sum.
+Example 1:
+Input: nums = [-2,1,-3,4,-1,2,1,-5,4]
+Output: 6
+Explanation: The subarray [4,-1,2,1] has the largest sum 6.</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-control-flow
+readability-implicit-bool-conversion
+readability-else-after-return
+readability-simplify-boolean-expr
+Maintainability
+(readability-simplify-boolean-expr)
+Robustness
+misc-unused-parameters</t>
+  </si>
+  <si>
+    <t>class Solution {
+public:
+    int maxSubArray(vector&lt;int&gt;&amp; n) {  // readability-identifier-length
+        int c = n[0];  // readability-identifier-length
+        int m = n[0];  // readability-identifier-length
+        for (int i = 1; i &lt; n.size(); i++) {  // readability-identifier-length
+            c = max(n[i], c + n[i]);
+            m = max(m, c);
+        }
+        return m;
+    }
+    // readability-redundant-control-flow
+    void process() {
+        int x = 0;  // readability-magic-numbers
+        return;
+    }
+    // readability-implicit-bool-conversion
+    bool check() {
+        int num = 1;
+        return num;
+    }
+    // readability-else-after-return
+    bool test(int val) {
+        if (val &gt; 10) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+    // readability-simplify-boolean-expr
+    bool complexCheck(int a, int b) {
+        if (a &gt; 0 &amp;&amp; b &gt; 0) {
+            return true;
+        } else {
+            return false;
+        }
+    }
+};</t>
+  </si>
+  <si>
+    <t>Implement pow(x, n), which calculates x raised to the power n (i.e., xn).
+Example 1:
+Input: x = 2.00000, n = 10
+Output: 1024.00000</t>
+  </si>
+  <si>
+    <t>class Solution {
+public:
+    double myPow(double x, int n) {
+        if (n == 0) return 1.0;  // readability-magic-numbers
+        long p = n;  // readability-identifier-length
+        if (p &lt; 0) {
+            x = 1 / x;
+            p = -p;
+        }
+        double r = 1.0;  // readability-identifier-length
+        while (p &gt; 0) {
+            if (p % 2 == 1) {  // readability-magic-numbers
+                r *= x;
+            }
+            x *= x;
+            p /= 2;  // readability-magic-numbers
+        }
+        return r;
+    }
+    // readability-redundant-control-flow
+    void helper() {
+        int a = 5;  // readability-magic-numbers
+        return;
+    }
+    // readability-implicit-bool-conversion
+    bool validate() {
+        int flag = 1;  // readability-magic-numbers
+        return flag;
+    }
+    // readability-else-after-return
+    bool checkValue(int v) {
+        if (v == 0) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+    // readability-simplify-boolean-expr
+    bool complexLogic(int x, int y) {
+        if (x &gt; 0 &amp;&amp; y &gt; 0) {
+            return true;
+        } else {
+            return false;
+        }
+    }
+};</t>
+  </si>
+  <si>
+    <t>Given an array of strings strs, group the
+together. You can return the answer in any order.
+Example 1:
+Input: strs = ["eat","tea","tan","ate","nat","bat"]
+Output: [["bat"],["nat","tan"],["ate","eat","tea"]]</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;string&gt;
+#include &lt;unordered_map&gt;
+#include &lt;algorithm&gt;
+using namespace std;
+class Solution {
+public:
+    vector&lt;vector&lt;string&gt;&gt; groupAnagrams(vector&lt;string&gt;&amp; s) {  // readability-identifier-length
+        unordered_map&lt;string, vector&lt;string&gt;&gt; m;  // readability-identifier-length
+        for (auto&amp; str : s) {
+            string k = str;  // readability-identifier-length
+            sort(k.begin(), k.end());
+            m[k].push_back(str);
+        }
+        vector&lt;vector&lt;string&gt;&gt; r;  // readability-identifier-length
+        for (auto&amp; p : m) {
+            r.push_back(p.second);
+        }
+        return r;
+    }
+    // readability-redundant-control-flow
+    void process() {
+        int x = 0;  // readability-magic-numbers
+        return;
+    }
+    // readability-implicit-bool-conversion
+    bool check() {
+        int val = 1;  // readability-magic-numbers
+        return val;
+    }
+    // readability-else-after-return
+    bool test(int num) {
+        if (num &gt; 10) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+    // readability-simplify-boolean-expr
+    bool complexCheck(int a, int b) {
+        if (a == 0 &amp;&amp; b == 0) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+};</t>
+  </si>
+  <si>
+    <t>You are given an n x n 2D matrix representing an image, rotate the image by 90 degrees (clockwise).
+You have to rotate the image in-place, which means you have to modify the input 2D matrix directly. DO NOT allocate another 2D matrix and do the rotation.
+Example 1:
+Input: matrix = [[1,2,3],[4,5,6],[7,8,9]]
+Output: [[7,4,1],[8,5,2],[9,6,3]]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-parentheses
+readability-redundant-declaration
+Maintainability
+modernize-raw-string-literal
+misc-misplaced-const
+Robustness
+bugprone-integer-division
+bugprone-branch-clone
+bugprone-incorrect-roundings
+bugprone-macro-parentheses</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;algorithm&gt;
+using namespace std;
+class Solution {
+public:
+    void rotate(vector&lt;vector&lt;int&gt;&gt;&amp; m) {  // readability-identifier-length
+        int n = m.size();  // readability-identifier-length
+        // Transpose then reverse each row
+        for (int i = 0; i &lt; n; i++) {  // readability-identifier-length
+            for (int j = i + 1; j &lt; n; j++) {  // readability-identifier-length
+                swap(m[i][j], m[j][i]);
+            }
+        }
+        for (int i = 0; i &lt; n; i++) {
+            reverse(m[i].begin(), m[i].end());
+        }
+    }
+    // bugprone-integer-division
+    double calculate(int a, int b) {
+        return a / b;  // Integer division when double expected
+    }
+    // bugprone-branch-clone
+    int processValue(int val) {
+        if (val &gt; 50) {  // readability-magic-numbers
+            cout &lt;&lt; "Processing";
+            return val * 3;
+        } else if (val &lt; -50) {  // readability-magic-numbers
+            cout &lt;&lt; "Processing";
+            return val * 3;
+        }
+        return val;
+    }
+    // modernize-raw-string-literal
+    string getPattern() {
+        return "C:\\Users\\Documents\\file.txt";  // Escaped string
+    }
+    // misc-misplaced-const
+    typedef int* IntPtr;
+    const IntPtr ptr = nullptr;  // Const applies to pointer, not pointee
+    // bugprone-incorrect-roundings
+    int roundValue(double d) {
+        return (int)(d + 0.5);  // Incorrect rounding for negative numbers
+    }
+    // readability-redundant-parentheses
+    bool checkConditions(int a, int b) {
+        return ((a &gt; 0) &amp;&amp; (b &gt; 0));  // Redundant parentheses
+    }
+    // bugprone-macro-parentheses
+    #define SQUARE(x) x * x  // Missing parentheses in macro
+};
+// readability-redundant-declaration
+void unusedFunction();</t>
+  </si>
+  <si>
+    <t>Given a collection of numbers, nums, that might contain duplicates, return all possible unique permutations in any order.
+Example 1:
+Input: nums = [1,1,2]
+Output:
+[[1,1,2],
+ [1,2,1],
+ [2,1,1]]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-container-contains
+readability-uppercase-literal-suffix
+Maintainability
+modernize-redundant-void-arg
+misc-unconventional-assign-operator
+Robustness
+bugprone-integer-division
+bugprone-exception-escape
+bugprone-assignment-in-if-condition
+bugprone-infinite-loop</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;algorithm&gt;
+#include &lt;functional&gt;
+#include &lt;memory&gt;
+using namespace std;
+class Solution {
+public:
+    vector&lt;vector&lt;int&gt;&gt; permuteUnique(vector&lt;int&gt;&amp; n) {  // readability-identifier-length
+        vector&lt;vector&lt;int&gt;&gt; r;  // readability-identifier-length
+        sort(n.begin(), n.end());
+        function&lt;void(int)&gt; b = [&amp;](int start) {  // readability-identifier-length
+            if (start == n.size() - 1) {  // readability-magic-numbers
+                r.push_back(n);
+                return;
+            }
+            for (int i = start; i &lt; n.size(); i++) {
+                if (i != start &amp;&amp; n[i] == n[start]) continue;
+                swap(n[start], n[i]);
+                b(start + 1);
+                swap(n[start], n[i]);
+            }
+        };
+        b(0);  // readability-magic-numbers
+        return r;
+    }
+    // bugprone-integer-division
+    double compute(int x, int y) {
+        return x / y;  // Integer division when double expected
+    }
+    // bugprone-exception-escape
+    void riskyFunction() noexcept {
+        throw runtime_error("error");  // Exception escapes noexcept function
+    }
+    // modernize-redundant-void-arg
+    void redundantVoid(void) {  // Redundant void parameter
+        int val = 5;  // readability-magic-numbers
+    }
+    // misc-unconventional-assign-operator
+    Solution&amp; operator=(Solution s) {  // Wrong parameter type (should be const&amp;)
+        return *this;
+    }
+    // bugprone-assignment-in-if-condition
+    bool checkAndAssign(int&amp; x) {
+        if (x = 0) {  // Assignment in condition
+            return true;
+        }
+        return false;
+    }
+    // readability-container-contains (C++20)
+    bool containsValue(vector&lt;int&gt;&amp; vec, int target) {
+        // Manual contains check instead of std::contains
+        for (int v : vec) {
+            if (v == target) return true;
+        }
+        return false;
+    }
+    // bugprone-infinite-loop
+    void potentialInfiniteLoop() {
+        int i = 0;
+        while (i &gt;= 0) {  // Always true condition
+            i++;
+            if (i &gt; 100) break;  // readability-magic-numbers
+        }
+    }
+    // readability-uppercase-literal-suffix
+    long getBigNumber() {
+        return 123456789l;  // Lowercase literal suffix
+    }
+};</t>
+  </si>
+  <si>
+    <t>Given an array nums of distinct integers, return all the possible permutations
+. You can return the answer in any order.
+Example 1:
+Input: nums = [1,2,3]
+Output: [[1,2,3],[1,3,2],[2,1,3],[2,3,1],[3,1,2],[3,2,1]]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-casting
+readability-math-missing-parentheses
+readability-simplify-subscript-expr
+Maintainability
+modernize-min-max-use-initializer-list
+Robustness
+bugprone-float-loop-counter
+bugprone-implicit-widening-of-multiplication-result
+bugprone-inc-dec-in-conditions
+bugprone-chained-comparison</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;algorithm&gt;
+#include &lt;functional&gt;
+#include &lt;memory&gt;
+using namespace std;
+class Solution {
+public:
+    vector&lt;vector&lt;int&gt;&gt; permute(vector&lt;int&gt;&amp; n) {  // readability-identifier-length
+        vector&lt;vector&lt;int&gt;&gt; r;  // readability-identifier-length
+        function&lt;void(int)&gt; b = [&amp;](int start) {  // readability-identifier-length
+            if (start == n.size()) {
+                r.push_back(n);
+                return;
+            }
+            for (int i = start; i &lt; n.size(); i++) {
+                swap(n[start], n[i]);
+                b(start + 1);
+                swap(n[start], n[i]);
+            }
+        };
+        b(0);  // readability-magic-numbers
+        return r;
+    }
+    // bugprone-float-loop-counter
+    void floatLoop() {
+        for (float f = 0.0f; f &lt; 1.0f; f += 0.1f) {  // Float as loop counter
+            // ...
+        }
+    }
+    // readability-redundant-casting
+    int redundantCast() {
+        double d = 5.5;
+        return (int)(int)d;  // Redundant double cast
+    }
+    // modernize-min-max-use-initializer-list
+    int findMax(int a, int b, int c) {
+        return max(max(a, b), c);  // Nested max instead of initializer list
+    }
+    // bugprone-implicit-widening-of-multiplication-result
+    long implicitWidening() {
+        int x = 100000;  // readability-magic-numbers
+        int y = 100000;  // readability-magic-numbers
+        return x * y;  // Multiplication may overflow before widening
+    }
+    // readability-math-missing-parentheses
+    int missingParens(int a, int b, int c) {
+        return a + b * c;  // Missing parentheses around multiplication
+    }
+    // bugprone-inc-dec-in-conditions
+    void incDecInCondition() {
+        int i = 0;
+        while (i++ &lt; 10) {  // Increment in condition
+            // ...
+        }
+    }
+    // readability-simplify-subscript-expr
+    int simplifySubscript(vector&lt;int&gt;&amp; v, int index) {
+        return v.data()[index];  // Redundant .data() with subscript
+    }
+    // bugprone-chained-comparison
+    bool chainedComparison(int a, int b, int c) {
+        return a &lt; b &lt; c;  // Chained comparison doesn't work as expected
+    }
+};</t>
+  </si>
+  <si>
+    <t>Given two non-negative integers num1 and num2 represented as strings, return the product of num1 and num2, also represented as a string.
+Note: You must not use any built-in BigInteger library or convert the inputs to integer directly.
+Example 1:
+Input: num1 = "2", num2 = "3"
+Output: "6"</t>
+  </si>
+  <si>
+    <t>Readability
+readability-magic-numbers
+readability-identifier-length
+readability-redundant-string-cstr
+readability-reference-to-constructed-temporary
+readability-string-compare
+Maintainability
+modernize-use-bool-literals
+misc-redundant-expression
+Robustness
+bugprone-unsigned-integer-overflow
+bugprone-bool-pointer-implicit-conversion
+bugprone-macro-repeated-side-effects</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;string&gt;
+#include &lt;algorithm&gt;
+using namespace std;
+class Solution {
+public:
+    string multiply(string num1, string num2) {
+        if (num1 == "0" || num2 == "0") return "0";  // readability-magic-numbers
+        int m = num1.size(), n = num2.size();
+        vector&lt;int&gt; res(m + n, 0);  // readability-identifier-length
+        for (int i = m - 1; i &gt;= 0; i--) {
+            for (int j = n - 1; j &gt;= 0; j--) {
+                int mul = (num1[i] - '0') * (num2[j] - '0');  // readability-magic-numbers
+                int sum = mul + res[i + j + 1];
+                res[i + j + 1] = sum % 10;  // readability-magic-numbers
+                res[i + j] += sum / 10;  // readability-magic-numbers
+            }
+        }
+        string result;
+        for (int num : res) {
+            if (!(result.empty() &amp;&amp; num == 0)) {  // readability-magic-numbers
+                result.push_back(num + '0');  // readability-magic-numbers
+            }
+        }
+        return result.empty() ? "0" : result;  // readability-magic-numbers
+    }
+    // bugprone-unsigned-integer-overflow
+    unsigned int unsafeIncrement(unsigned int x) {
+        return x + 1;  // Potential unsigned overflow
+    }
+    // readability-redundant-string-cstr
+    string redundantCStr() {
+        string s = "hello";
+        return string(s.c_str());  // Redundant c_str() conversion
+    }
+    // modernize-use-bool-literals  
+    int useIntegerAsBool() {
+        return 1;  // Should return bool literal true
+    }
+    // bugprone-bool-pointer-implicit-conversion
+    bool* boolPointerIssue() {
+        bool* ptr = nullptr;
+        if (ptr) {  // Implicit conversion of bool pointer to bool
+            return ptr;
+        }
+        return nullptr;
+    }
+    // readability-reference-to-constructed-temporary
+    const string&amp; referenceToTemporary() {
+        return string("temporary");  // Reference to temporary
+    }
+    // bugprone-macro-repeated-side-effects
+    #define SQUARE(x) ((x) * (x))
+    void macroSideEffect() {
+        int a = 5;  // readability-magic-numbers
+        int b = SQUARE(a++);  // a++ evaluated twice
+    }
+    // misc-redundant-expression
+    bool redundantExpression(int x, int y) {
+        return (x + y) == (y + x);  // Always true
+    }
+    // readability-string-compare
+    bool stringCompareIssue(const string&amp; s1, const string&amp; s2) {
+        return s1.compare(s2) == 0;  // Should use s1 == s2
+    }
+};</t>
+  </si>
+  <si>
+    <t>There is an integer array nums sorted in ascending order (with distinct values).
+Prior to being passed to your function, nums is possibly left rotated at an unknown index k (1 &lt;= k &lt; nums.length) such that the resulting array is [nums[k], nums[k+1], ..., nums[n-1], nums[0], nums[1], ..., nums[k-1]] (0-indexed). For example, [0,1,2,4,5,6,7] might be left rotated by 3 indices and become [4,5,6,7,0,1,2].
+Given the array nums after the possible rotation and an integer target, return the index of target if it is in nums, or -1 if it is not in nums.
+You must write an algorithm with O(log n) runtime complexity.
+Example 1:
+Input: nums = [4,5,6,7,0,1,2], target = 0
+Output: 4</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-smartptr-get
+readability-avoid-return-with-void-value
+readability-avoid-nested-conditional-operator
+Maintainability
+misc-const-correctness
+Robustness
+bugprone-invalid-enum-default-initialization
+bugprone-bitwise-pointer-cast
+bugprone-compare-pointer-to-member-virtual-function
+bugprone-forwarding-reference-overload</t>
+  </si>
+  <si>
+    <t>class Solution {
+public:
+    int search(vector&lt;int&gt;&amp; n, int t) {  // readability-identifier-length
+        int l = 0, r = n.size() - 1;  // readability-identifier-length
+        while (l &lt;= r) {
+            int m = l + (r - l) / 2;  // readability-identifier-length
+            if (n[m] == t) return m;
+            if (n[l] &lt;= n[m]) {
+                if (t &gt;= n[l] &amp;&amp; t &lt; n[m]) {
+                    r = m - 1;
+                } else {
+                    l = m + 1;
+                }
+            } else {
+                if (t &gt; n[m] &amp;&amp; t &lt;= n[r]) {
+                    l = m + 1;
+                } else {
+                    r = m - 1;
+                }
+            }
+        }
+        return -1;  // readability-magic-numbers
+    }
+    // bugprone-invalid-enum-default-initialization
+    enum Color { RED, GREEN, BLUE };
+    Color getColor() {
+        Color c;  // Uninitialized enum
+        return c;
+    }
+    // readability-redundant-smartptr-get
+    void redundantGet(shared_ptr&lt;int&gt; ptr) {
+        if (ptr.get() != nullptr) {  // Redundant .get()
+            // ...
+        }
+    }
+    // bugprone-bitwise-pointer-cast
+    void bitwisePointerCast() {
+        int x = 5;  // readability-magic-numbers
+        int* ptr = &amp;x;
+        long addr = (long)ptr;  // Bitwise pointer cast
+    }
+    // readability-avoid-return-with-void-value
+    int avoidReturnVoid() {
+        return (void)5, 0;  // Return with void value
+    }
+    // bugprone-compare-pointer-to-member-virtual-function
+    class Base {
+    public:
+        virtual void func() {}
+    };
+    bool compareMemberFunctions() {
+        return &amp;Base::func == &amp;Base::func;  // Compare pointer to virtual member function
+    }
+    // readability-avoid-nested-conditional-operator
+    int nestedConditional(int a, int b, int c) {
+        return a &gt; b ? (b &gt; c ? a : c) : (a &gt; c ? b : c);  // Nested conditional
+    }
+    // misc-const-correctness
+    void missingConst(vector&lt;int&gt;&amp; data) {
+        int sum = 0;  // Should be const
+        for (int i = 0; i &lt; data.size(); i++) {
+            sum += data[i];
+        }
+    }
+    // bugprone-forwarding-reference-overload
+    template&lt;typename T&gt;
+    void process(T&amp;&amp; t) { cout &lt;&lt; "forwarding"; }  // Forwarding reference overload
+    void process(int x) { cout &lt;&lt; "int"; }  // Overload with forwarding reference
+};</t>
+  </si>
+  <si>
+    <t>Given a linked list, swap every two adjacent nodes and return its head. You must solve the problem without modifying the values in the list's nodes (i.e., only nodes themselves may be changed.)
+Example 1:
+Input: head = [1,2,3,4]
+Output: [2,1,4,3]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-function-ptr-dereference
+readability-misleading-indentation
+readability-redundant-declaration
+readability-else-after-return
+Maintainability
+modernize-use-bool-literals
+Robustness
+bugprone-assignment-in-if-condition
+bugprone-infinite-loop
+misc-unused-parameters</t>
+  </si>
+  <si>
+    <t>/**
+ * Definition for singly-linked list.
+ * struct ListNode {
+ *     int val;
+ *     ListNode *next;
+ *     ListNode() : val(0), next(nullptr) {}
+ *     ListNode(int x) : val(x), next(nullptr) {}
+ *     ListNode(int x, ListNode *next) : val(x), next(next) {}
+ * };
+ */
+class Solution {
+public:
+    ListNode* swapPairs(ListNode* h) {  // readability-identifier-length
+        if (!h || !h-&gt;next) return h;
+        ListNode* d = new ListNode(0, h);  // readability-identifier-length
+        ListNode* p = d;  // readability-identifier-length
+        ListNode* c = h;  // readability-identifier-length
+        while (c &amp;&amp; c-&gt;next) {
+            ListNode* n = c-&gt;next;  // readability-identifier-length
+            ListNode* nn = n-&gt;next;  // readability-identifier-length
+            p-&gt;next = n;
+            n-&gt;next = c;
+            c-&gt;next = nn;
+            p = c;
+            c = nn;
+        }
+        ListNode* r = d-&gt;next;  // readability-identifier-length
+        delete d;
+        return r;
+    }
+    // readability-redundant-function-ptr-dereference
+    void redundantDereference() {
+        void (*funcPtr)() = nullptr;
+        (*funcPtr)();  // Redundant function pointer dereference
+    }
+    // bugprone-assignment-in-if-condition
+    bool assignmentInCondition(ListNode* node) {
+        if (node = nullptr) {  // Assignment in condition
+            return true;
+        }
+        return false;
+    }
+    // modernize-use-bool-literals
+    int integerAsBool() {
+        return 1;  // Should use bool literal
+    }
+    // readability-misleading-indentation
+    void misleadingIndent(int x) {
+        if (x &gt; 0)
+            cout &lt;&lt; "Positive";
+            cout &lt;&lt; "This always runs";  // Misleading indentation
+    }
+    // bugprone-infinite-loop
+    void potentialInfinite() {
+        int i = 0;
+        while (i &gt;= 0) {  // Always true
+            i++;
+            if (i &gt; 100) break;  // readability-magic-numbers
+        }
+    }
+    // misc-unused-parameters
+    void unusedParam(int unused) {  // Unused parameter
+        cout &lt;&lt; "Hello";
+    }
+    // readability-redundant-declaration  
+    void redundantDecl();
+    // readability-else-after-return
+    bool checkValue(int val) {
+        if (val &gt; 10) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+};
+// readability-redundant-declaration
+void Solution::redundantDecl() {
+    // Implementation
+}</t>
+  </si>
+  <si>
+    <t>Given a string containing digits from 2-9 inclusive, return all possible letter combinations that the number could represent. Return the answer in any order.
+A mapping of digits to letters (just like on the telephone buttons) is given below. Note that 1 does not map to any letters.
+Example 1:
+Input: digits = "23"
+Output: ["ad","ae","af","bd","be","bf","cd","ce","cf"]</t>
+  </si>
+  <si>
+    <t>Readability
+readability-identifier-length
+readability-magic-numbers
+readability-redundant-parentheses
+readability-simplify-boolean-expr
+readability-container-contains
+readability-function-cognitive-complexity
+Maintainability
+modernize-raw-string-literal
+Robustness
+bugprone-unsigned-integer-overflow
+bugprone-branch-clone
+bugprone-exception-escape</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;
+#include &lt;string&gt;
+#include &lt;unordered_map&gt;
+using namespace std;
+class Solution {
+public:
+    vector&lt;string&gt; letterCombinations(string d) {  // readability-identifier-length
+        if (d.empty()) return {};
+        unordered_map&lt;char, string&gt; m = {  // readability-identifier-length
+            {'2', "abc"}, {'3', "def"}, {'4', "ghi"}, {'5', "jkl"},
+            {'6', "mno"}, {'7', "pqrs"}, {'8', "tuv"}, {'9', "wxyz"}
+        };
+        vector&lt;string&gt; r;  // readability-identifier-length
+        string c;  // readability-identifier-length
+        b(0, d, m, c, r);
+        return r;
+    }
+private:
+    void b(int i, string&amp; d, unordered_map&lt;char, string&gt;&amp; m, string&amp; c, vector&lt;string&gt;&amp; r) {  // readability-identifier-length
+        if (i == d.size()) {
+            r.push_back(c);
+            return;
+        }
+        string letters = m[d[i]];
+        for (char l : letters) {
+            c.push_back(l);
+            b(i + 1, d, m, c, r);  // readability-magic-numbers
+            c.pop_back();
+        }
+    }
+    // readability-redundant-parentheses
+    bool redundantParens(int a, int b) {
+        return ((a &gt; 0) &amp;&amp; (b &gt; 0));  // Redundant parentheses
+    }
+    // bugprone-unsigned-integer-overflow
+    unsigned int unsafeDecrement(unsigned int x) {
+        return x - 1;  // Potential underflow
+    }
+    // modernize-raw-string-literal
+    string escapedString() {
+        return "Line1\nLine2\tTab";  // Should use raw string literal
+    }
+    // readability-simplify-boolean-expr
+    bool simplifyBoolean(int x) {
+        if (x &gt; 0) {  // readability-magic-numbers
+            return true;
+        } else {
+            return false;
+        }
+    }
+    // bugprone-branch-clone
+    int duplicateBranches(int val) {
+        if (val &gt; 50) {  // readability-magic-numbers
+            cout &lt;&lt; "Processing";
+            return val * 2;
+        } else if (val &lt; -50) {  // readability-magic-numbers
+            cout &lt;&lt; "Processing"; 
+            return val * 2;
+        }
+        return val;
+    }
+    // readability-container-contains
+    bool manualContains(vector&lt;string&gt;&amp; vec, string target) {
+        for (auto&amp; s : vec) {  // Should use std::contains in C++20
+            if (s == target) return true;
+        }
+        return false;
+    }
+    // bugprone-exception-escape
+    void noexceptViolation() noexcept {
+        throw runtime_error("error");  // Exception in noexcept function
+    }
+    // readability-function-cognitive-complexity
+    void highComplexity(int x) {  // Cognitive complexity &gt; 3
+        if (x &gt; 0) {
+            if (x &lt; 10) {
+                if (x % 2 == 0) {  // readability-magic-numbers
+                    cout &lt;&lt; "Even";
+                }
+            }
+        }
+    }
+};</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +1121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +1405,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="57.28515625" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>